<commit_message>
COGMENTO-1238 Working on Contacts class: removed .0 from zip, birthDay and birthYear
</commit_message>
<xml_diff>
--- a/target/classes/contactData/CogmentoTestData.xlsx
+++ b/target/classes/contactData/CogmentoTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="15020" tabRatio="500"/>
+    <workbookView windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="333">
   <si>
     <t>firstname</t>
   </si>
@@ -209,7 +209,7 @@
     <t>Some Identifier</t>
   </si>
   <si>
-    <t>src/main/resources/images/image.png</t>
+    <t>src/main/resources/images/1.png</t>
   </si>
   <si>
     <t>John</t>
@@ -668,7 +668,7 @@
     <t>March</t>
   </si>
   <si>
-    <t>src/main/resources/images/7.jpg</t>
+    <t>src/main/resources/images/1.jpg</t>
   </si>
   <si>
     <t>Sweeney</t>
@@ -721,9 +721,6 @@
     <t>Data scientist</t>
   </si>
   <si>
-    <t>src/main/resources/images/8.jpg</t>
-  </si>
-  <si>
     <t>Christina</t>
   </si>
   <si>
@@ -780,9 +777,6 @@
     <t>September</t>
   </si>
   <si>
-    <t>src/main/resources/images/9.jpg</t>
-  </si>
-  <si>
     <t>Britney</t>
   </si>
   <si>
@@ -833,9 +827,6 @@
     <t>Computer scientist</t>
   </si>
   <si>
-    <t>src/main/resources/images/10.jpg</t>
-  </si>
-  <si>
     <t>Spacey</t>
   </si>
   <si>
@@ -886,9 +877,6 @@
     <t>Cloud system engineer</t>
   </si>
   <si>
-    <t>src/main/resources/images/11.jpg</t>
-  </si>
-  <si>
     <t>Tim</t>
   </si>
   <si>
@@ -942,9 +930,6 @@
     <t>April</t>
   </si>
   <si>
-    <t>src/main/resources/images/12.jpg</t>
-  </si>
-  <si>
     <t>Uma</t>
   </si>
   <si>
@@ -1001,9 +986,6 @@
     <t>August</t>
   </si>
   <si>
-    <t>src/main/resources/images/13.jpg</t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
@@ -1060,9 +1042,6 @@
     <t>February</t>
   </si>
   <si>
-    <t>src/main/resources/images/14.jpg</t>
-  </si>
-  <si>
     <t>Morgan</t>
   </si>
   <si>
@@ -1116,9 +1095,6 @@
     <t>Applications engineer</t>
   </si>
   <si>
-    <t>src/main/resources/images/15.jpg</t>
-  </si>
-  <si>
     <t>Deni</t>
   </si>
   <si>
@@ -1169,9 +1145,6 @@
     <t>15555</t>
   </si>
   <si>
-    <t>src/main/resources/images/16.jpg</t>
-  </si>
-  <si>
     <t>Haruki</t>
   </si>
   <si>
@@ -1219,9 +1192,6 @@
     <t>16666</t>
   </si>
   <si>
-    <t>src/main/resources/images/17.jpg</t>
-  </si>
-  <si>
     <t>Lev</t>
   </si>
   <si>
@@ -1272,9 +1242,6 @@
     <t>17777</t>
   </si>
   <si>
-    <t>src/main/resources/images/18.jpg</t>
-  </si>
-  <si>
     <t>Dmitri</t>
   </si>
   <si>
@@ -1325,9 +1292,6 @@
     <t>18888</t>
   </si>
   <si>
-    <t>src/main/resources/images/19.jpg</t>
-  </si>
-  <si>
     <t>Smith</t>
   </si>
   <si>
@@ -1375,9 +1339,6 @@
     <t>19999</t>
   </si>
   <si>
-    <t>src/main/resources/images/20.jpg</t>
-  </si>
-  <si>
     <t>cal</t>
   </si>
 </sst>
@@ -1387,8 +1348,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -1417,33 +1378,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1454,44 +1392,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1507,17 +1417,39 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1529,9 +1461,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1539,6 +1478,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1553,10 +1499,25 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1569,31 +1530,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1611,7 +1584,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1623,13 +1662,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1641,19 +1680,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1665,91 +1698,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1793,15 +1754,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1817,26 +1769,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1858,6 +1795,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1867,11 +1815,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1880,134 +1841,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2362,8 +2323,8 @@
   <sheetPr/>
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AJ21" sqref="AJ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0078125" defaultRowHeight="14"/>
@@ -3378,21 +3339,21 @@
         <v>62</v>
       </c>
       <c r="AJ9" s="8" t="s">
-        <v>194</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>40</v>
@@ -3401,7 +3362,7 @@
         <v>148</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>96</v>
@@ -3413,28 +3374,28 @@
         <v>98</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>123</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N10" s="2">
         <v>8</v>
       </c>
       <c r="O10" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="P10" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>78</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>52</v>
@@ -3449,10 +3410,10 @@
         <v>128</v>
       </c>
       <c r="W10" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="X10" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="Y10" s="2" t="s">
         <v>130</v>
@@ -3479,7 +3440,7 @@
         <v>31</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AH10" s="2">
         <v>1973</v>
@@ -3488,21 +3449,21 @@
         <v>62</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>208</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>40</v>
@@ -3511,7 +3472,7 @@
         <v>168</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>43</v>
@@ -3523,28 +3484,28 @@
         <v>121</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N11" s="2">
         <v>8</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>166</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>52</v>
@@ -3559,7 +3520,7 @@
         <v>54</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="X11" s="8" t="s">
         <v>149</v>
@@ -3598,7 +3559,7 @@
         <v>62</v>
       </c>
       <c r="AJ11" s="8" t="s">
-        <v>220</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:36">
@@ -3606,13 +3567,13 @@
         <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>40</v>
@@ -3621,7 +3582,7 @@
         <v>180</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>70</v>
@@ -3633,28 +3594,28 @@
         <v>141</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>47</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="N12" s="2">
         <v>8</v>
       </c>
       <c r="O12" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="R12" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>52</v>
@@ -3669,10 +3630,10 @@
         <v>54</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y12" s="2" t="s">
         <v>56</v>
@@ -3708,21 +3669,21 @@
         <v>62</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>232</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
@@ -3731,7 +3692,7 @@
         <v>193</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>96</v>
@@ -3743,25 +3704,25 @@
         <v>161</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>74</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="N13" s="2">
         <v>8</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>104</v>
@@ -3779,10 +3740,10 @@
         <v>54</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y13" s="2" t="s">
         <v>83</v>
@@ -3809,7 +3770,7 @@
         <v>12</v>
       </c>
       <c r="AG13" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="AH13" s="2">
         <v>1972</v>
@@ -3818,30 +3779,30 @@
         <v>62</v>
       </c>
       <c r="AJ13" s="8" t="s">
-        <v>245</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>43</v>
@@ -3853,28 +3814,28 @@
         <v>45</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="N14" s="2">
         <v>8</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>52</v>
@@ -3889,7 +3850,7 @@
         <v>106</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>82</v>
@@ -3919,7 +3880,7 @@
         <v>26</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AH14" s="2">
         <v>1959</v>
@@ -3928,30 +3889,30 @@
         <v>62</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>259</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:36">
       <c r="A15" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>70</v>
@@ -3963,28 +3924,28 @@
         <v>72</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>123</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="N15" s="2">
         <v>8</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>52</v>
@@ -3999,10 +3960,10 @@
         <v>128</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y15" s="2" t="s">
         <v>130</v>
@@ -4029,7 +3990,7 @@
         <v>27</v>
       </c>
       <c r="AG15" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AH15" s="2">
         <v>1983</v>
@@ -4038,30 +3999,30 @@
         <v>62</v>
       </c>
       <c r="AJ15" s="8" t="s">
-        <v>273</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:36">
       <c r="A16" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>96</v>
@@ -4073,28 +4034,28 @@
         <v>98</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="N16" s="2">
         <v>8</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>52</v>
@@ -4109,7 +4070,7 @@
         <v>54</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="X16" s="8" t="s">
         <v>149</v>
@@ -4148,30 +4109,30 @@
         <v>62</v>
       </c>
       <c r="AJ16" s="2" t="s">
-        <v>286</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:36">
       <c r="A17" s="3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>43</v>
@@ -4183,28 +4144,28 @@
         <v>121</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="N17" s="2">
         <v>8</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>52</v>
@@ -4222,7 +4183,7 @@
         <v>41</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>56</v>
@@ -4249,7 +4210,7 @@
         <v>19</v>
       </c>
       <c r="AG17" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="AH17" s="2">
         <v>1995</v>
@@ -4258,30 +4219,30 @@
         <v>62</v>
       </c>
       <c r="AJ17" s="8" t="s">
-        <v>298</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:36">
       <c r="A18" s="3" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>70</v>
@@ -4293,28 +4254,28 @@
         <v>141</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="N18" s="2">
         <v>8</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>166</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>52</v>
@@ -4332,7 +4293,7 @@
         <v>68</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y18" s="2" t="s">
         <v>83</v>
@@ -4368,30 +4329,30 @@
         <v>62</v>
       </c>
       <c r="AJ18" s="2" t="s">
-        <v>309</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:36">
       <c r="A19" s="3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>43</v>
@@ -4403,28 +4364,28 @@
         <v>161</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="N19" s="2">
         <v>8</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>52</v>
@@ -4469,7 +4430,7 @@
         <v>3</v>
       </c>
       <c r="AG19" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AH19" s="2">
         <v>1970</v>
@@ -4478,30 +4439,30 @@
         <v>62</v>
       </c>
       <c r="AJ19" s="8" t="s">
-        <v>321</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:36">
       <c r="A20" s="3" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>70</v>
@@ -4513,28 +4474,28 @@
         <v>45</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>123</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="N20" s="2">
         <v>8</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>52</v>
@@ -4552,7 +4513,7 @@
         <v>118</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y20" s="2" t="s">
         <v>130</v>
@@ -4588,7 +4549,7 @@
         <v>62</v>
       </c>
       <c r="AJ20" s="2" t="s">
-        <v>333</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:36">
@@ -4596,22 +4557,22 @@
         <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>96</v>
@@ -4623,28 +4584,28 @@
         <v>45</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>143</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="N21" s="2">
         <v>8</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>166</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>52</v>
@@ -4689,7 +4650,7 @@
         <v>21</v>
       </c>
       <c r="AG21" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AH21" s="2">
         <v>1972</v>
@@ -4698,7 +4659,7 @@
         <v>62</v>
       </c>
       <c r="AJ21" s="8" t="s">
-        <v>344</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4746,7 +4707,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>